<commit_message>
basic regresion testing with responsive metrics
</commit_message>
<xml_diff>
--- a/covid-19_dist0720 .xlsx
+++ b/covid-19_dist0720 .xlsx
@@ -1,30 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaJiD\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaepark/MIDS/W203/Lab-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53B6952-108E-45D8-90AC-19F6F9DAD040}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A6086E-C203-4649-9D66-B42CC517D919}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Infromation" sheetId="1" r:id="rId1"/>
     <sheet name="Covid-19" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -311,7 +303,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+  </numFmts>
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,6 +452,20 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -858,21 +867,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -916,6 +910,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1273,20 +1278,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" customWidth="1"/>
-    <col min="2" max="2" width="49.109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="37.77734375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="49.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" style="8" customWidth="1"/>
     <col min="4" max="4" width="18" style="8" customWidth="1"/>
-    <col min="5" max="5" width="31.77734375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1301,17 +1306,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="40.799999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:8" ht="40.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="18">
         <v>44014</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -1321,145 +1326,145 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="20"/>
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="7"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="20"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="21"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="7"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="20"/>
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="21"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="7"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="21"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="7"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
+    <row r="7" spans="1:8" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="21"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="7"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:8" ht="100.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="21"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="7"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="21"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="7"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="21"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="7"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
+    <row r="11" spans="1:8" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="21"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="7"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="7"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
+    <row r="13" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
       <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="7"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1468,17 +1473,17 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="25" t="s">
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="17">
         <v>2018</v>
       </c>
       <c r="E15" s="7"/>
@@ -1486,67 +1491,67 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
       <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="7"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="20"/>
       <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
       <c r="E17" s="7"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
+    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
       <c r="B18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="7"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
+    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
       <c r="B19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="7"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
       <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="7"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1555,84 +1560,84 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="16">
         <v>44018</v>
       </c>
-      <c r="E22" s="19"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
-      <c r="B23" s="15" t="s">
+    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="21"/>
+      <c r="B23" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="19"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
-      <c r="B24" s="15" t="s">
+    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="21"/>
+      <c r="B24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="19"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="14"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="15" t="s">
+    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="21"/>
+      <c r="B25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="19"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
-      <c r="B26" s="15" t="s">
+    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="21"/>
+      <c r="B26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="19"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="14"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="27"/>
-      <c r="B27" s="20" t="s">
+    <row r="27" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="12">
         <v>44017</v>
       </c>
-      <c r="E27" s="16"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1662,20 +1667,22 @@
   <dimension ref="A1:Y53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" customWidth="1"/>
     <col min="10" max="10" width="22.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="9" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="9" customFormat="1" ht="110" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>35</v>
       </c>
@@ -1694,7 +1701,7 @@
       <c r="F1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="13" t="s">
         <v>89</v>
       </c>
       <c r="H1" s="9" t="s">
@@ -1752,7 +1759,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1774,22 +1781,22 @@
       <c r="G2">
         <v>449886</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="25">
         <v>43903</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="26">
         <v>43925</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="27">
         <v>43951</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="26">
         <v>43918</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="27">
         <v>43951</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="26">
         <v>43962</v>
       </c>
       <c r="N2">
@@ -1829,7 +1836,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1851,22 +1858,22 @@
       <c r="G3">
         <v>122732</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="25">
         <v>43901</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="26">
         <v>43918</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="27">
         <v>43945</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="26">
         <v>43918</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="27">
         <v>43945</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="26">
         <v>43945</v>
       </c>
       <c r="N3">
@@ -1906,7 +1913,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1928,22 +1935,22 @@
       <c r="G4">
         <v>604362</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="25">
         <v>43901</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="26">
         <v>43921</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="27">
         <v>43967</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="26">
         <v>43920</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="27">
         <v>43959</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="26">
         <v>43959</v>
       </c>
       <c r="N4">
@@ -1983,7 +1990,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -2005,22 +2012,22 @@
       <c r="G5">
         <v>604362</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="25">
         <v>43901</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="26">
         <v>43921</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="27">
         <v>43967</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="26">
         <v>43920</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="27">
         <v>43959</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="26">
         <v>43959</v>
       </c>
       <c r="N5">
@@ -2060,7 +2067,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -2082,22 +2089,22 @@
       <c r="G6">
         <v>338893</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="25">
         <v>43901</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="28">
+        <v>43913</v>
+      </c>
+      <c r="J6" s="27">
         <v>0</v>
       </c>
-      <c r="J6" s="14">
-        <v>0</v>
-      </c>
-      <c r="K6" s="11">
-        <v>0</v>
-      </c>
-      <c r="L6" s="13">
+      <c r="K6" s="26">
+        <v>43925</v>
+      </c>
+      <c r="L6" s="27">
         <v>43955</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="26">
         <v>43962</v>
       </c>
       <c r="N6">
@@ -2137,7 +2144,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -2159,22 +2166,22 @@
       <c r="G7">
         <v>4680138</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="25">
         <v>43894</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="26">
         <v>43909</v>
       </c>
-      <c r="J7" s="14">
-        <v>0</v>
-      </c>
-      <c r="K7" s="10">
+      <c r="J7" s="27">
+        <v>43959</v>
+      </c>
+      <c r="K7" s="26">
         <v>43909</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="27">
         <v>43959</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="26">
         <v>43956</v>
       </c>
       <c r="N7">
@@ -2214,7 +2221,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -2236,22 +2243,22 @@
       <c r="G8">
         <v>350717</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="25">
         <v>43901</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="26">
         <v>43916</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="27">
         <v>43948</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="26">
         <v>43916</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="27">
         <v>43952</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="26">
         <v>43944</v>
       </c>
       <c r="N8">
@@ -2291,7 +2298,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2313,22 +2320,22 @@
       <c r="G9">
         <v>499669</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="25">
         <v>43900</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="29">
+        <v>43913</v>
+      </c>
+      <c r="J9" s="27">
         <v>0</v>
       </c>
-      <c r="J9" s="14">
-        <v>0</v>
-      </c>
-      <c r="K9" s="10">
+      <c r="K9" s="26">
         <v>43913</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="27">
         <v>43971</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="26">
         <v>43924</v>
       </c>
       <c r="N9">
@@ -2368,7 +2375,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -2390,22 +2397,22 @@
       <c r="G10">
         <v>123941</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="25">
         <v>43903</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="26">
         <v>43914</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="27">
         <v>43983</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="26">
         <v>43914</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="27">
         <v>43959</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="26">
         <v>43952</v>
       </c>
       <c r="N10">
@@ -2445,7 +2452,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -2467,22 +2474,22 @@
       <c r="G11">
         <v>105993</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="25">
         <v>43901</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="26">
         <v>43922</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="27">
         <v>43980</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="26">
         <v>43915</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="27">
         <v>43980</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="26">
         <v>43936</v>
       </c>
       <c r="N11">
@@ -2522,7 +2529,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -2544,22 +2551,22 @@
       <c r="G12">
         <v>2200199</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="25">
         <v>43899</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="26">
         <v>43924</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="27">
         <v>43969</v>
       </c>
-      <c r="K12" s="11">
-        <v>0</v>
-      </c>
-      <c r="L12" s="13">
+      <c r="K12" s="26">
+        <v>43909</v>
+      </c>
+      <c r="L12" s="27">
         <v>43969</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="26">
         <v>43962</v>
       </c>
       <c r="N12">
@@ -2599,7 +2606,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -2621,22 +2628,22 @@
       <c r="G13">
         <v>949185</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="25">
         <v>43904</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="26">
         <v>43924</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="27">
         <v>43952</v>
       </c>
-      <c r="K13" s="11">
-        <v>0</v>
-      </c>
-      <c r="L13" s="13">
+      <c r="K13" s="26">
+        <v>43924</v>
+      </c>
+      <c r="L13" s="27">
         <v>43952</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="26">
         <v>43948</v>
       </c>
       <c r="N13">
@@ -2676,7 +2683,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -2698,22 +2705,22 @@
       <c r="G14">
         <v>84325</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="25">
         <v>43894</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="26">
         <v>43915</v>
       </c>
-      <c r="J14" s="14">
-        <v>0</v>
-      </c>
-      <c r="K14" s="10">
+      <c r="J14" s="27">
+        <v>43958</v>
+      </c>
+      <c r="K14" s="26">
         <v>43915</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="27">
         <v>43958</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="26">
         <v>43937</v>
       </c>
       <c r="N14">
@@ -2753,7 +2760,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -2775,22 +2782,22 @@
       <c r="G15">
         <v>104266</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="25">
         <v>43903</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="26">
         <v>43915</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="27">
         <v>43952</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="26">
         <v>43915</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="27">
         <v>43952</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="26">
         <v>0</v>
       </c>
       <c r="N15">
@@ -2830,7 +2837,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -2852,22 +2859,22 @@
       <c r="G16">
         <v>1762828</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="25">
         <v>43899</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="26">
         <v>43911</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="27">
         <v>43980</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="26">
         <v>43911</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="27">
         <v>43980</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="26">
         <v>43952</v>
       </c>
       <c r="N16">
@@ -2907,7 +2914,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -2929,22 +2936,22 @@
       <c r="G17">
         <v>521722</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="25">
         <v>43896</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="26">
         <v>43915</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="27">
         <v>43969</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="26">
         <v>43915</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="27">
         <v>43969</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="26">
         <v>43952</v>
       </c>
       <c r="N17">
@@ -2984,7 +2991,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -3006,22 +3013,22 @@
       <c r="G18">
         <v>332472</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="25">
         <v>43899</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="26">
         <v>0</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="27">
         <v>0</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="26">
         <v>43916</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="27">
         <v>43966</v>
       </c>
-      <c r="M18" s="11">
+      <c r="M18" s="26">
         <v>0</v>
       </c>
       <c r="N18">
@@ -3061,7 +3068,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -3083,22 +3090,22 @@
       <c r="G19">
         <v>191561</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="25">
         <v>43902</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="26">
         <v>43920</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="27">
         <v>43955</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="26">
         <v>43920</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="27">
         <v>43955</v>
       </c>
-      <c r="M19" s="11">
+      <c r="M19" s="26">
         <v>0</v>
       </c>
       <c r="N19">
@@ -3138,7 +3145,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -3157,22 +3164,22 @@
       <c r="F20">
         <v>366.5</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="25">
         <v>43896</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="26">
         <v>0</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="27">
         <v>0</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="26">
         <v>43916</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="27">
         <v>43962</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="26">
         <v>43962</v>
       </c>
       <c r="N20">
@@ -3212,7 +3219,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -3234,22 +3241,22 @@
       <c r="G21">
         <v>802454</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="25">
         <v>43901</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="26">
         <v>43913</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="27">
         <v>43966</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="26">
         <v>43913</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="27">
         <v>43952</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="26">
         <v>43952</v>
       </c>
       <c r="N21">
@@ -3289,7 +3296,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -3311,22 +3318,22 @@
       <c r="G22">
         <v>107932</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="25">
         <v>43905</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="26">
         <v>43922</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="27">
         <v>43982</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="26">
         <v>43915</v>
       </c>
-      <c r="L22" s="13">
+      <c r="L22" s="27">
         <v>43952</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="26">
         <v>43952</v>
       </c>
       <c r="N22">
@@ -3366,7 +3373,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -3388,22 +3395,22 @@
       <c r="G23">
         <v>579962</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="25">
         <v>43895</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="26">
         <v>43920</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="27">
         <v>43966</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="26">
         <v>43913</v>
       </c>
-      <c r="L23" s="13">
+      <c r="L23" s="27">
         <v>43966</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="26">
         <v>43939</v>
       </c>
       <c r="N23">
@@ -3443,7 +3450,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -3465,22 +3472,22 @@
       <c r="G24">
         <v>891685</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="25">
         <v>43900</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="26">
         <v>43914</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="27">
         <v>43969</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="26">
         <v>43914</v>
       </c>
-      <c r="L24" s="13">
+      <c r="L24" s="27">
         <v>43969</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24" s="26">
         <v>43957</v>
       </c>
       <c r="N24">
@@ -3520,7 +3527,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -3542,22 +3549,22 @@
       <c r="G25">
         <v>1146819</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="25">
         <v>43900</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="26">
         <v>43914</v>
       </c>
-      <c r="J25" s="13">
+      <c r="J25" s="27">
         <v>43983</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="26">
         <v>43914</v>
       </c>
-      <c r="L25" s="13">
+      <c r="L25" s="27">
         <v>43977</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="26">
         <v>43947</v>
       </c>
       <c r="N25">
@@ -3597,7 +3604,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -3619,22 +3626,22 @@
       <c r="G26">
         <v>674015</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="25">
         <v>43903</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="26">
         <v>43918</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="27">
         <v>43969</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="26">
         <v>43918</v>
       </c>
-      <c r="L26" s="13">
+      <c r="L26" s="27">
         <v>43948</v>
       </c>
-      <c r="M26" s="10">
+      <c r="M26" s="26">
         <v>43983</v>
       </c>
       <c r="N26">
@@ -3674,7 +3681,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -3696,22 +3703,22 @@
       <c r="G27">
         <v>310141</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H27" s="25">
         <v>43904</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27" s="26">
         <v>43924</v>
       </c>
-      <c r="J27" s="13">
+      <c r="J27" s="27">
         <v>43948</v>
       </c>
-      <c r="K27" s="10">
+      <c r="K27" s="26">
         <v>43924</v>
       </c>
-      <c r="L27" s="13">
+      <c r="L27" s="27">
         <v>43948</v>
       </c>
-      <c r="M27" s="10">
+      <c r="M27" s="26">
         <v>43958</v>
       </c>
       <c r="N27">
@@ -3751,7 +3758,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -3773,22 +3780,22 @@
       <c r="G28">
         <v>419509</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="25">
         <v>43903</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="26">
         <v>43927</v>
       </c>
-      <c r="J28" s="13">
+      <c r="J28" s="27">
         <v>43955</v>
       </c>
-      <c r="K28" s="11">
-        <v>0</v>
-      </c>
-      <c r="L28" s="13">
+      <c r="K28" s="26">
+        <v>43927</v>
+      </c>
+      <c r="L28" s="27">
         <v>43955</v>
       </c>
-      <c r="M28" s="11">
+      <c r="M28" s="26">
         <v>0</v>
       </c>
       <c r="N28">
@@ -3828,7 +3835,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -3850,22 +3857,22 @@
       <c r="G29">
         <v>100106</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="25">
         <v>43902</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="26">
         <v>43918</v>
       </c>
-      <c r="J29" s="13">
+      <c r="J29" s="27">
         <v>43947</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="26">
         <v>43918</v>
       </c>
-      <c r="L29" s="13">
+      <c r="L29" s="27">
         <v>43948</v>
       </c>
-      <c r="M29" s="11">
+      <c r="M29" s="26">
         <v>0</v>
       </c>
       <c r="N29">
@@ -3905,7 +3912,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -3927,22 +3934,22 @@
       <c r="G30">
         <v>189928</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H30" s="25">
         <v>43903</v>
       </c>
-      <c r="I30" s="11">
+      <c r="I30" s="26">
         <v>0</v>
       </c>
-      <c r="J30" s="14">
+      <c r="J30" s="27">
         <v>0</v>
       </c>
-      <c r="K30" s="11">
-        <v>0</v>
-      </c>
-      <c r="L30" s="13">
+      <c r="K30" s="26">
+        <v>43924</v>
+      </c>
+      <c r="L30" s="27">
         <v>43969</v>
       </c>
-      <c r="M30" s="10">
+      <c r="M30" s="26">
         <v>43955</v>
       </c>
       <c r="N30">
@@ -3982,7 +3989,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -4004,22 +4011,22 @@
       <c r="G31">
         <v>307697</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="25">
         <v>43902</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="26">
         <v>43921</v>
       </c>
-      <c r="J31" s="13">
+      <c r="J31" s="27">
         <v>43960</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K31" s="26">
         <v>43911</v>
       </c>
-      <c r="L31" s="13">
+      <c r="L31" s="27">
         <v>43960</v>
       </c>
-      <c r="M31" s="10">
+      <c r="M31" s="26">
         <v>43960</v>
       </c>
       <c r="N31">
@@ -4059,7 +4066,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -4081,22 +4088,22 @@
       <c r="G32">
         <v>123749</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="25">
         <v>43903</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="26">
         <v>43918</v>
       </c>
-      <c r="J32" s="13">
+      <c r="J32" s="27">
         <v>43998</v>
       </c>
-      <c r="K32" s="10">
+      <c r="K32" s="26">
         <v>43918</v>
       </c>
-      <c r="L32" s="13">
+      <c r="L32" s="27">
         <v>43962</v>
       </c>
-      <c r="M32" s="10">
+      <c r="M32" s="26">
         <v>43952</v>
       </c>
       <c r="N32">
@@ -4136,7 +4143,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -4158,22 +4165,22 @@
       <c r="G33">
         <v>1534640</v>
       </c>
-      <c r="H33" s="12">
+      <c r="H33" s="25">
         <v>43899</v>
       </c>
-      <c r="I33" s="11">
+      <c r="I33" s="28">
+        <v>43913</v>
+      </c>
+      <c r="J33" s="26">
         <v>0</v>
       </c>
-      <c r="J33" s="11">
-        <v>0</v>
-      </c>
-      <c r="K33" s="10">
+      <c r="K33" s="26">
         <v>43911</v>
       </c>
-      <c r="L33" s="13">
+      <c r="L33" s="27">
         <v>43969</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M33" s="26">
         <v>43929</v>
       </c>
       <c r="N33">
@@ -4213,7 +4220,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -4235,22 +4242,22 @@
       <c r="G34">
         <v>372288</v>
       </c>
-      <c r="H34" s="12">
+      <c r="H34" s="25">
         <v>43901</v>
       </c>
-      <c r="I34" s="10">
+      <c r="I34" s="26">
         <v>43914</v>
       </c>
-      <c r="J34" s="14">
-        <v>0</v>
-      </c>
-      <c r="K34" s="10">
+      <c r="J34" s="27">
+        <v>44027</v>
+      </c>
+      <c r="K34" s="26">
         <v>43914</v>
       </c>
-      <c r="L34" s="13">
+      <c r="L34" s="27">
         <v>43966</v>
       </c>
-      <c r="M34" s="10">
+      <c r="M34" s="26">
         <v>43957</v>
       </c>
       <c r="N34">
@@ -4290,7 +4297,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -4312,22 +4319,22 @@
       <c r="G35">
         <v>4233803</v>
       </c>
-      <c r="H35" s="12">
+      <c r="H35" s="25">
         <v>43897</v>
       </c>
-      <c r="I35" s="10">
+      <c r="I35" s="26">
         <v>43912</v>
       </c>
-      <c r="J35" s="14">
-        <v>0</v>
-      </c>
-      <c r="K35" s="10">
+      <c r="J35" s="27">
+        <v>44009</v>
+      </c>
+      <c r="K35" s="26">
         <v>43912</v>
       </c>
-      <c r="L35" s="13">
+      <c r="L35" s="27">
         <v>43966</v>
       </c>
-      <c r="M35" s="10">
+      <c r="M35" s="26">
         <v>43938</v>
       </c>
       <c r="N35">
@@ -4367,7 +4374,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -4389,22 +4396,22 @@
       <c r="G36">
         <v>1036838</v>
       </c>
-      <c r="H36" s="12">
+      <c r="H36" s="25">
         <v>43900</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I36" s="26">
         <v>43920</v>
       </c>
-      <c r="J36" s="13">
+      <c r="J36" s="27">
         <v>43973</v>
       </c>
-      <c r="K36" s="10">
+      <c r="K36" s="26">
         <v>43920</v>
       </c>
-      <c r="L36" s="13">
+      <c r="L36" s="27">
         <v>43959</v>
       </c>
-      <c r="M36" s="10">
+      <c r="M36" s="26">
         <v>44008</v>
       </c>
       <c r="N36">
@@ -4444,7 +4451,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -4466,22 +4473,22 @@
       <c r="G37">
         <v>113128</v>
       </c>
-      <c r="H37" s="12">
+      <c r="H37" s="25">
         <v>43903</v>
       </c>
-      <c r="I37" s="11">
+      <c r="I37" s="26">
         <v>0</v>
       </c>
-      <c r="J37" s="14">
+      <c r="J37" s="27">
         <v>0</v>
       </c>
-      <c r="K37" s="11">
-        <v>0</v>
-      </c>
-      <c r="L37" s="13">
+      <c r="K37" s="26">
+        <v>43917</v>
+      </c>
+      <c r="L37" s="27">
         <v>43952</v>
       </c>
-      <c r="M37" s="10">
+      <c r="M37" s="26">
         <v>43949</v>
       </c>
       <c r="N37">
@@ -4521,7 +4528,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -4543,22 +4550,22 @@
       <c r="G38">
         <v>868762</v>
       </c>
-      <c r="H38" s="12">
+      <c r="H38" s="25">
         <v>43899</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I38" s="26">
         <v>43914</v>
       </c>
-      <c r="J38" s="13">
+      <c r="J38" s="27">
         <v>43971</v>
       </c>
-      <c r="K38" s="10">
+      <c r="K38" s="26">
         <v>43914</v>
       </c>
-      <c r="L38" s="13">
+      <c r="L38" s="27">
         <v>43955</v>
       </c>
-      <c r="M38" s="10">
+      <c r="M38" s="26">
         <v>43950</v>
       </c>
       <c r="N38">
@@ -4589,7 +4596,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -4611,22 +4618,22 @@
       <c r="G39">
         <v>364717</v>
       </c>
-      <c r="H39" s="12">
+      <c r="H39" s="25">
         <v>43905</v>
       </c>
-      <c r="I39" s="11">
+      <c r="I39" s="26">
         <v>0</v>
       </c>
-      <c r="J39" s="14">
+      <c r="J39" s="27">
         <v>0</v>
       </c>
-      <c r="K39" s="10">
+      <c r="K39" s="26">
         <v>43922</v>
       </c>
-      <c r="L39" s="13">
+      <c r="L39" s="27">
         <v>43945</v>
       </c>
-      <c r="M39" s="11">
+      <c r="M39" s="26">
         <v>0</v>
       </c>
       <c r="N39">
@@ -4666,7 +4673,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -4688,22 +4695,22 @@
       <c r="G40">
         <v>264201</v>
       </c>
-      <c r="H40" s="12">
+      <c r="H40" s="25">
         <v>43898</v>
       </c>
-      <c r="I40" s="10">
+      <c r="I40" s="26">
         <v>43913</v>
       </c>
-      <c r="J40" s="13">
+      <c r="J40" s="27">
         <v>44001</v>
       </c>
-      <c r="K40" s="11">
-        <v>0</v>
-      </c>
-      <c r="L40" s="13">
+      <c r="K40" s="26">
+        <v>43913</v>
+      </c>
+      <c r="L40" s="27">
         <v>43966</v>
       </c>
-      <c r="M40" s="10">
+      <c r="M40" s="26">
         <v>43960</v>
       </c>
       <c r="N40">
@@ -4743,7 +4750,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -4765,22 +4772,22 @@
       <c r="G41">
         <v>824700</v>
       </c>
-      <c r="H41" s="12">
+      <c r="H41" s="25">
         <v>43896</v>
       </c>
-      <c r="I41" s="10">
+      <c r="I41" s="26">
         <v>43922</v>
       </c>
-      <c r="J41" s="13">
+      <c r="J41" s="27">
         <v>43987</v>
       </c>
-      <c r="K41" s="10">
+      <c r="K41" s="26">
         <v>43909</v>
       </c>
-      <c r="L41" s="13">
+      <c r="L41" s="27">
         <v>43987</v>
       </c>
-      <c r="M41" s="10">
+      <c r="M41" s="26">
         <v>43940</v>
       </c>
       <c r="N41">
@@ -4820,7 +4827,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -4842,22 +4849,22 @@
       <c r="G42">
         <v>250954</v>
       </c>
-      <c r="H42" s="12">
+      <c r="H42" s="25">
         <v>43899</v>
       </c>
-      <c r="I42" s="10">
+      <c r="I42" s="26">
         <v>43918</v>
       </c>
-      <c r="J42" s="13">
+      <c r="J42" s="27">
         <v>43960</v>
       </c>
-      <c r="K42" s="10">
+      <c r="K42" s="26">
         <v>43920</v>
       </c>
-      <c r="L42" s="13">
+      <c r="L42" s="27">
         <v>43960</v>
       </c>
-      <c r="M42" s="10">
+      <c r="M42" s="26">
         <v>43939</v>
       </c>
       <c r="N42">
@@ -4897,7 +4904,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>76</v>
       </c>
@@ -4919,22 +4926,22 @@
       <c r="G43">
         <v>430809</v>
       </c>
-      <c r="H43" s="12">
+      <c r="H43" s="25">
         <v>43903</v>
       </c>
-      <c r="I43" s="10">
+      <c r="I43" s="26">
         <v>43928</v>
       </c>
-      <c r="J43" s="13">
+      <c r="J43" s="27">
         <v>43955</v>
       </c>
-      <c r="K43" s="10">
+      <c r="K43" s="26">
         <v>43922</v>
       </c>
-      <c r="L43" s="13">
+      <c r="L43" s="27">
         <v>43941</v>
       </c>
-      <c r="M43" s="11">
+      <c r="M43" s="26">
         <v>0</v>
       </c>
       <c r="N43">
@@ -4974,7 +4981,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>77</v>
       </c>
@@ -4996,22 +5003,22 @@
       <c r="G44">
         <v>84003</v>
       </c>
-      <c r="H44" s="12">
+      <c r="H44" s="25">
         <v>43903</v>
       </c>
-      <c r="I44" s="11">
+      <c r="I44" s="26">
         <v>0</v>
       </c>
-      <c r="J44" s="14">
+      <c r="J44" s="27">
         <v>0</v>
       </c>
-      <c r="K44" s="11">
+      <c r="K44" s="26">
         <v>0</v>
       </c>
-      <c r="L44" s="14">
+      <c r="L44" s="27">
         <v>0</v>
       </c>
-      <c r="M44" s="11">
+      <c r="M44" s="26">
         <v>0</v>
       </c>
       <c r="N44">
@@ -5051,7 +5058,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>78</v>
       </c>
@@ -5073,22 +5080,22 @@
       <c r="G45">
         <v>896166</v>
       </c>
-      <c r="H45" s="12">
+      <c r="H45" s="25">
         <v>43902</v>
       </c>
-      <c r="I45" s="10">
+      <c r="I45" s="26">
         <v>43923</v>
       </c>
-      <c r="J45" s="13">
+      <c r="J45" s="27">
         <v>43952</v>
       </c>
-      <c r="K45" s="10">
+      <c r="K45" s="26">
         <v>43922</v>
       </c>
-      <c r="L45" s="13">
+      <c r="L45" s="27">
         <v>43952</v>
       </c>
-      <c r="M45" s="11">
+      <c r="M45" s="26">
         <v>0</v>
       </c>
       <c r="N45">
@@ -5128,7 +5135,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>79</v>
       </c>
@@ -5150,22 +5157,22 @@
       <c r="G46">
         <v>2133457</v>
       </c>
-      <c r="H46" s="12">
+      <c r="H46" s="25">
         <v>43903</v>
       </c>
-      <c r="I46" s="11">
+      <c r="I46" s="29">
+        <v>43923</v>
+      </c>
+      <c r="J46" s="27">
         <v>0</v>
       </c>
-      <c r="J46" s="14">
-        <v>0</v>
-      </c>
-      <c r="K46" s="10">
+      <c r="K46" s="26">
         <v>43921</v>
       </c>
-      <c r="L46" s="13">
+      <c r="L46" s="27">
         <v>43952</v>
       </c>
-      <c r="M46" s="10">
+      <c r="M46" s="26">
         <v>43959</v>
       </c>
       <c r="N46">
@@ -5205,7 +5212,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>80</v>
       </c>
@@ -5227,22 +5234,22 @@
       <c r="G47">
         <v>371308</v>
       </c>
-      <c r="H47" s="12">
+      <c r="H47" s="25">
         <v>43896</v>
       </c>
-      <c r="I47" s="11">
+      <c r="I47" s="26">
         <v>0</v>
       </c>
-      <c r="J47" s="14">
+      <c r="J47" s="27">
         <v>0</v>
       </c>
-      <c r="K47" s="11">
-        <v>0</v>
-      </c>
-      <c r="L47" s="13">
+      <c r="K47" s="26">
+        <v>43919</v>
+      </c>
+      <c r="L47" s="27">
         <v>43952</v>
       </c>
-      <c r="M47" s="10">
+      <c r="M47" s="26">
         <v>43931</v>
       </c>
       <c r="N47">
@@ -5282,7 +5289,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>81</v>
       </c>
@@ -5304,22 +5311,22 @@
       <c r="G48">
         <v>70024</v>
       </c>
-      <c r="H48" s="12">
+      <c r="H48" s="25">
         <v>43903</v>
       </c>
-      <c r="I48" s="10">
+      <c r="I48" s="26">
         <v>43915</v>
       </c>
-      <c r="J48" s="13">
+      <c r="J48" s="27">
         <v>43966</v>
       </c>
-      <c r="K48" s="10">
+      <c r="K48" s="26">
         <v>43915</v>
       </c>
-      <c r="L48" s="13">
+      <c r="L48" s="27">
         <v>43948</v>
       </c>
-      <c r="M48" s="10">
+      <c r="M48" s="26">
         <v>43938</v>
       </c>
       <c r="N48">
@@ -5359,7 +5366,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>82</v>
       </c>
@@ -5381,22 +5388,22 @@
       <c r="G49">
         <v>709355</v>
       </c>
-      <c r="H49" s="12">
+      <c r="H49" s="25">
         <v>43902</v>
       </c>
-      <c r="I49" s="10">
+      <c r="I49" s="26">
         <v>43920</v>
       </c>
-      <c r="J49" s="13">
+      <c r="J49" s="27">
         <v>43980</v>
       </c>
-      <c r="K49" s="11">
-        <v>0</v>
-      </c>
-      <c r="L49" s="13">
+      <c r="K49" s="26">
+        <v>43914</v>
+      </c>
+      <c r="L49" s="27">
         <v>43980</v>
       </c>
-      <c r="M49" s="10">
+      <c r="M49" s="26">
         <v>43980</v>
       </c>
       <c r="N49">
@@ -5436,7 +5443,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>83</v>
       </c>
@@ -5458,22 +5465,22 @@
       <c r="G50">
         <v>607276</v>
       </c>
-      <c r="H50" s="12">
+      <c r="H50" s="25">
         <v>43890</v>
       </c>
-      <c r="I50" s="10">
+      <c r="I50" s="26">
         <v>43913</v>
       </c>
-      <c r="J50" s="13">
+      <c r="J50" s="27">
         <v>43983</v>
       </c>
-      <c r="K50" s="10">
+      <c r="K50" s="26">
         <v>43915</v>
       </c>
-      <c r="L50" s="13">
+      <c r="L50" s="27">
         <v>43956</v>
       </c>
-      <c r="M50" s="10">
+      <c r="M50" s="26">
         <v>43955</v>
       </c>
       <c r="N50">
@@ -5513,7 +5520,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>84</v>
       </c>
@@ -5535,22 +5542,22 @@
       <c r="G51">
         <v>184821</v>
       </c>
-      <c r="H51" s="12">
+      <c r="H51" s="25">
         <v>43906</v>
       </c>
-      <c r="I51" s="10">
+      <c r="I51" s="26">
         <v>43914</v>
       </c>
-      <c r="J51" s="13">
+      <c r="J51" s="27">
         <v>43955</v>
       </c>
-      <c r="K51" s="10">
+      <c r="K51" s="26">
         <v>43914</v>
       </c>
-      <c r="L51" s="13">
+      <c r="L51" s="27">
         <v>43955</v>
       </c>
-      <c r="M51" s="10">
+      <c r="M51" s="26">
         <v>43955</v>
       </c>
       <c r="N51">
@@ -5590,7 +5597,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -5612,22 +5619,22 @@
       <c r="G52">
         <v>618851</v>
       </c>
-      <c r="H52" s="12">
+      <c r="H52" s="25">
         <v>43902</v>
       </c>
-      <c r="I52" s="10">
+      <c r="I52" s="26">
         <v>43915</v>
       </c>
-      <c r="J52" s="13">
+      <c r="J52" s="27">
         <v>43964</v>
       </c>
-      <c r="K52" s="10">
+      <c r="K52" s="26">
         <v>43915</v>
       </c>
-      <c r="L52" s="13">
+      <c r="L52" s="27">
         <v>43962</v>
       </c>
-      <c r="M52" s="11">
+      <c r="M52" s="26">
         <v>0</v>
       </c>
       <c r="N52">
@@ -5667,7 +5674,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>86</v>
       </c>
@@ -5689,22 +5696,22 @@
       <c r="G53">
         <v>35327</v>
       </c>
-      <c r="H53" s="12">
+      <c r="H53" s="25">
         <v>43903</v>
       </c>
-      <c r="I53" s="11">
+      <c r="I53" s="26">
         <v>0</v>
       </c>
-      <c r="J53" s="14">
+      <c r="J53" s="27">
         <v>0</v>
       </c>
-      <c r="K53" s="11">
-        <v>0</v>
-      </c>
-      <c r="L53" s="13">
+      <c r="K53" s="26">
+        <v>43914</v>
+      </c>
+      <c r="L53" s="27">
         <v>43952</v>
       </c>
-      <c r="M53" s="10">
+      <c r="M53" s="26">
         <v>43952</v>
       </c>
       <c r="N53">

</xml_diff>